<commit_message>
update xuất file và trường hợp chief là người đánh giá
</commit_message>
<xml_diff>
--- a/assets/templates/HDTV.xlsx
+++ b/assets/templates/HDTV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\khanhmf\Project_Flutter\LabourContract\web_labor_contract\assets\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD Kang/WebLabor/WebLabor/assets/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA2DBC3-B909-45B3-AC6E-CBD62EB0874A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E3D3B-D354-5F4E-B730-B70A19BD9778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C11091E5-9F21-408F-A1BD-137C6D20AAD6}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19720" xr2:uid="{C11091E5-9F21-408F-A1BD-137C6D20AAD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>Phụ biểu 1
 付表 1</t>
@@ -391,6 +390,9 @@
   <si>
     <t xml:space="preserve">Ngày/日:   </t>
   </si>
+  <si>
+    <t>Chief xác nhận kết quả đánh giá Chiefが評価結果を確認</t>
+  </si>
 </sst>
 </file>
 
@@ -742,7 +744,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -796,19 +798,25 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -880,17 +888,14 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1228,152 +1233,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D5B744-72E8-4AB2-8660-D8EB4CF29633}">
-  <dimension ref="A1:AA159"/>
+  <dimension ref="A1:AB159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="F7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="14.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" style="1" customWidth="1"/>
-    <col min="12" max="13" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="1"/>
+    <col min="10" max="10" width="14.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="11.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="13" style="1" customWidth="1"/>
     <col min="15" max="17" width="9" style="1" customWidth="1"/>
-    <col min="18" max="18" width="8.5703125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8.28515625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="8.33203125" style="1" customWidth="1"/>
     <col min="20" max="20" width="9" style="1" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="9.83203125" style="1" customWidth="1"/>
     <col min="22" max="22" width="11" style="1" customWidth="1"/>
     <col min="23" max="23" width="10" style="1" customWidth="1"/>
     <col min="24" max="24" width="10" style="2" customWidth="1"/>
-    <col min="25" max="25" width="11.85546875" style="2" customWidth="1"/>
-    <col min="26" max="26" width="9.5703125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="11.83203125" style="2" customWidth="1"/>
+    <col min="26" max="26" width="9.5" style="2" customWidth="1"/>
     <col min="27" max="27" width="18" style="2" customWidth="1"/>
     <col min="28" max="38" width="18" style="1" customWidth="1"/>
-    <col min="39" max="75" width="16.28515625" style="1" customWidth="1"/>
-    <col min="76" max="16384" width="9.140625" style="1"/>
+    <col min="39" max="75" width="16.33203125" style="1" customWidth="1"/>
+    <col min="76" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-    </row>
-    <row r="4" spans="1:27" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+    </row>
+    <row r="4" spans="1:28" ht="37" x14ac:dyDescent="0.15">
+      <c r="A4" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-    </row>
-    <row r="6" spans="1:27" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
+      <c r="U4" s="60"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="60"/>
+      <c r="X4" s="60"/>
+      <c r="Y4" s="60"/>
+      <c r="Z4" s="60"/>
+    </row>
+    <row r="6" spans="1:28" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.15">
+      <c r="A6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="G6" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="31" t="s">
+      <c r="J6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="31" t="s">
+      <c r="K6" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="34" t="s">
+      <c r="L6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="35" t="s">
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="36"/>
-      <c r="U6" s="36"/>
-      <c r="V6" s="36"/>
-      <c r="W6" s="36"/>
-      <c r="X6" s="36"/>
-      <c r="Y6" s="36"/>
-      <c r="Z6" s="36"/>
-      <c r="AA6" s="37"/>
-    </row>
-    <row r="7" spans="1:27" s="8" customFormat="1" ht="198" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="38"/>
+      <c r="W6" s="38"/>
+      <c r="X6" s="38"/>
+      <c r="Y6" s="38"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="39"/>
+    </row>
+    <row r="7" spans="1:28" s="8" customFormat="1" ht="180" x14ac:dyDescent="0.2">
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
       <c r="L7" s="5" t="s">
         <v>15</v>
       </c>
@@ -1422,8 +1427,11 @@
       <c r="AA7" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB7" s="61" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -1475,8 +1483,9 @@
       <c r="AA8" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB8" s="10"/>
+    </row>
+    <row r="9" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="11"/>
@@ -1504,8 +1513,9 @@
       <c r="Y9" s="15"/>
       <c r="Z9" s="15"/>
       <c r="AA9" s="16"/>
-    </row>
-    <row r="10" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB9" s="10"/>
+    </row>
+    <row r="10" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -1533,8 +1543,9 @@
       <c r="Y10" s="15"/>
       <c r="Z10" s="15"/>
       <c r="AA10" s="16"/>
-    </row>
-    <row r="11" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB10" s="10"/>
+    </row>
+    <row r="11" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
@@ -1562,8 +1573,9 @@
       <c r="Y11" s="15"/>
       <c r="Z11" s="15"/>
       <c r="AA11" s="16"/>
-    </row>
-    <row r="12" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB11" s="10"/>
+    </row>
+    <row r="12" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="10"/>
       <c r="C12" s="11"/>
@@ -1591,8 +1603,9 @@
       <c r="Y12" s="15"/>
       <c r="Z12" s="15"/>
       <c r="AA12" s="16"/>
-    </row>
-    <row r="13" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB12" s="10"/>
+    </row>
+    <row r="13" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="10"/>
       <c r="C13" s="11"/>
@@ -1620,8 +1633,9 @@
       <c r="Y13" s="15"/>
       <c r="Z13" s="15"/>
       <c r="AA13" s="16"/>
-    </row>
-    <row r="14" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB13" s="10"/>
+    </row>
+    <row r="14" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
@@ -1649,8 +1663,9 @@
       <c r="Y14" s="15"/>
       <c r="Z14" s="15"/>
       <c r="AA14" s="16"/>
-    </row>
-    <row r="15" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB14" s="10"/>
+    </row>
+    <row r="15" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
       <c r="C15" s="11"/>
@@ -1678,8 +1693,9 @@
       <c r="Y15" s="15"/>
       <c r="Z15" s="15"/>
       <c r="AA15" s="16"/>
-    </row>
-    <row r="16" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB15" s="10"/>
+    </row>
+    <row r="16" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
@@ -1707,8 +1723,9 @@
       <c r="Y16" s="15"/>
       <c r="Z16" s="15"/>
       <c r="AA16" s="16"/>
-    </row>
-    <row r="17" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB16" s="10"/>
+    </row>
+    <row r="17" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
       <c r="C17" s="11"/>
@@ -1736,8 +1753,9 @@
       <c r="Y17" s="15"/>
       <c r="Z17" s="15"/>
       <c r="AA17" s="16"/>
-    </row>
-    <row r="18" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB17" s="10"/>
+    </row>
+    <row r="18" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
@@ -1765,8 +1783,9 @@
       <c r="Y18" s="15"/>
       <c r="Z18" s="15"/>
       <c r="AA18" s="16"/>
-    </row>
-    <row r="19" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB18" s="10"/>
+    </row>
+    <row r="19" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="11"/>
@@ -1794,8 +1813,9 @@
       <c r="Y19" s="15"/>
       <c r="Z19" s="15"/>
       <c r="AA19" s="16"/>
-    </row>
-    <row r="20" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB19" s="10"/>
+    </row>
+    <row r="20" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="10"/>
       <c r="C20" s="11"/>
@@ -1823,8 +1843,9 @@
       <c r="Y20" s="15"/>
       <c r="Z20" s="15"/>
       <c r="AA20" s="16"/>
-    </row>
-    <row r="21" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB20" s="10"/>
+    </row>
+    <row r="21" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="11"/>
@@ -1852,8 +1873,9 @@
       <c r="Y21" s="15"/>
       <c r="Z21" s="15"/>
       <c r="AA21" s="16"/>
-    </row>
-    <row r="22" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB21" s="10"/>
+    </row>
+    <row r="22" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="11"/>
@@ -1881,8 +1903,9 @@
       <c r="Y22" s="15"/>
       <c r="Z22" s="15"/>
       <c r="AA22" s="16"/>
-    </row>
-    <row r="23" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB22" s="10"/>
+    </row>
+    <row r="23" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -1910,8 +1933,9 @@
       <c r="Y23" s="15"/>
       <c r="Z23" s="15"/>
       <c r="AA23" s="16"/>
-    </row>
-    <row r="24" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB23" s="10"/>
+    </row>
+    <row r="24" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="11"/>
@@ -1939,8 +1963,9 @@
       <c r="Y24" s="15"/>
       <c r="Z24" s="15"/>
       <c r="AA24" s="16"/>
-    </row>
-    <row r="25" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB24" s="10"/>
+    </row>
+    <row r="25" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
       <c r="C25" s="11"/>
@@ -1968,8 +1993,9 @@
       <c r="Y25" s="15"/>
       <c r="Z25" s="15"/>
       <c r="AA25" s="16"/>
-    </row>
-    <row r="26" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB25" s="10"/>
+    </row>
+    <row r="26" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
@@ -1997,8 +2023,9 @@
       <c r="Y26" s="15"/>
       <c r="Z26" s="15"/>
       <c r="AA26" s="16"/>
-    </row>
-    <row r="27" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB26" s="10"/>
+    </row>
+    <row r="27" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="10"/>
       <c r="C27" s="11"/>
@@ -2026,8 +2053,9 @@
       <c r="Y27" s="15"/>
       <c r="Z27" s="15"/>
       <c r="AA27" s="16"/>
-    </row>
-    <row r="28" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB27" s="10"/>
+    </row>
+    <row r="28" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="10"/>
       <c r="C28" s="11"/>
@@ -2055,8 +2083,9 @@
       <c r="Y28" s="15"/>
       <c r="Z28" s="15"/>
       <c r="AA28" s="16"/>
-    </row>
-    <row r="29" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB28" s="10"/>
+    </row>
+    <row r="29" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="10"/>
       <c r="C29" s="11"/>
@@ -2084,8 +2113,9 @@
       <c r="Y29" s="15"/>
       <c r="Z29" s="15"/>
       <c r="AA29" s="16"/>
-    </row>
-    <row r="30" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB29" s="10"/>
+    </row>
+    <row r="30" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="10"/>
       <c r="C30" s="11"/>
@@ -2113,8 +2143,9 @@
       <c r="Y30" s="15"/>
       <c r="Z30" s="15"/>
       <c r="AA30" s="16"/>
-    </row>
-    <row r="31" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB30" s="10"/>
+    </row>
+    <row r="31" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
       <c r="C31" s="11"/>
@@ -2142,8 +2173,9 @@
       <c r="Y31" s="15"/>
       <c r="Z31" s="15"/>
       <c r="AA31" s="16"/>
-    </row>
-    <row r="32" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB31" s="10"/>
+    </row>
+    <row r="32" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
@@ -2171,8 +2203,9 @@
       <c r="Y32" s="15"/>
       <c r="Z32" s="15"/>
       <c r="AA32" s="16"/>
-    </row>
-    <row r="33" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB32" s="10"/>
+    </row>
+    <row r="33" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="10"/>
       <c r="C33" s="11"/>
@@ -2200,8 +2233,9 @@
       <c r="Y33" s="15"/>
       <c r="Z33" s="15"/>
       <c r="AA33" s="16"/>
-    </row>
-    <row r="34" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB33" s="10"/>
+    </row>
+    <row r="34" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
       <c r="B34" s="10"/>
       <c r="C34" s="11"/>
@@ -2229,8 +2263,9 @@
       <c r="Y34" s="15"/>
       <c r="Z34" s="15"/>
       <c r="AA34" s="16"/>
-    </row>
-    <row r="35" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB34" s="10"/>
+    </row>
+    <row r="35" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="10"/>
       <c r="C35" s="11"/>
@@ -2258,8 +2293,9 @@
       <c r="Y35" s="15"/>
       <c r="Z35" s="15"/>
       <c r="AA35" s="16"/>
-    </row>
-    <row r="36" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB35" s="10"/>
+    </row>
+    <row r="36" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="10"/>
       <c r="C36" s="11"/>
@@ -2287,8 +2323,9 @@
       <c r="Y36" s="15"/>
       <c r="Z36" s="15"/>
       <c r="AA36" s="16"/>
-    </row>
-    <row r="37" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB36" s="10"/>
+    </row>
+    <row r="37" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
@@ -2316,8 +2353,9 @@
       <c r="Y37" s="15"/>
       <c r="Z37" s="15"/>
       <c r="AA37" s="16"/>
-    </row>
-    <row r="38" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB37" s="10"/>
+    </row>
+    <row r="38" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
       <c r="B38" s="10"/>
       <c r="C38" s="11"/>
@@ -2345,8 +2383,9 @@
       <c r="Y38" s="15"/>
       <c r="Z38" s="15"/>
       <c r="AA38" s="16"/>
-    </row>
-    <row r="39" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB38" s="10"/>
+    </row>
+    <row r="39" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="10"/>
       <c r="C39" s="11"/>
@@ -2374,8 +2413,9 @@
       <c r="Y39" s="15"/>
       <c r="Z39" s="15"/>
       <c r="AA39" s="16"/>
-    </row>
-    <row r="40" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB39" s="10"/>
+    </row>
+    <row r="40" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
       <c r="B40" s="10"/>
       <c r="C40" s="11"/>
@@ -2403,8 +2443,9 @@
       <c r="Y40" s="15"/>
       <c r="Z40" s="15"/>
       <c r="AA40" s="16"/>
-    </row>
-    <row r="41" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB40" s="10"/>
+    </row>
+    <row r="41" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
       <c r="B41" s="10"/>
       <c r="C41" s="11"/>
@@ -2432,8 +2473,9 @@
       <c r="Y41" s="15"/>
       <c r="Z41" s="15"/>
       <c r="AA41" s="16"/>
-    </row>
-    <row r="42" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB41" s="10"/>
+    </row>
+    <row r="42" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
       <c r="B42" s="10"/>
       <c r="C42" s="11"/>
@@ -2461,8 +2503,9 @@
       <c r="Y42" s="15"/>
       <c r="Z42" s="15"/>
       <c r="AA42" s="16"/>
-    </row>
-    <row r="43" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB42" s="10"/>
+    </row>
+    <row r="43" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
       <c r="B43" s="10"/>
       <c r="C43" s="11"/>
@@ -2490,8 +2533,9 @@
       <c r="Y43" s="15"/>
       <c r="Z43" s="15"/>
       <c r="AA43" s="16"/>
-    </row>
-    <row r="44" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB43" s="10"/>
+    </row>
+    <row r="44" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
       <c r="B44" s="10"/>
       <c r="C44" s="11"/>
@@ -2519,8 +2563,9 @@
       <c r="Y44" s="15"/>
       <c r="Z44" s="15"/>
       <c r="AA44" s="16"/>
-    </row>
-    <row r="45" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB44" s="10"/>
+    </row>
+    <row r="45" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
       <c r="B45" s="10"/>
       <c r="C45" s="11"/>
@@ -2548,8 +2593,9 @@
       <c r="Y45" s="15"/>
       <c r="Z45" s="15"/>
       <c r="AA45" s="16"/>
-    </row>
-    <row r="46" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB45" s="10"/>
+    </row>
+    <row r="46" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
@@ -2577,8 +2623,9 @@
       <c r="Y46" s="15"/>
       <c r="Z46" s="15"/>
       <c r="AA46" s="16"/>
-    </row>
-    <row r="47" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB46" s="10"/>
+    </row>
+    <row r="47" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
       <c r="B47" s="10"/>
       <c r="C47" s="11"/>
@@ -2606,8 +2653,9 @@
       <c r="Y47" s="15"/>
       <c r="Z47" s="15"/>
       <c r="AA47" s="16"/>
-    </row>
-    <row r="48" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB47" s="10"/>
+    </row>
+    <row r="48" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
       <c r="B48" s="10"/>
       <c r="C48" s="11"/>
@@ -2635,8 +2683,9 @@
       <c r="Y48" s="15"/>
       <c r="Z48" s="15"/>
       <c r="AA48" s="16"/>
-    </row>
-    <row r="49" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB48" s="10"/>
+    </row>
+    <row r="49" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="9"/>
       <c r="B49" s="10"/>
       <c r="C49" s="11"/>
@@ -2664,8 +2713,9 @@
       <c r="Y49" s="15"/>
       <c r="Z49" s="15"/>
       <c r="AA49" s="16"/>
-    </row>
-    <row r="50" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB49" s="10"/>
+    </row>
+    <row r="50" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
       <c r="B50" s="10"/>
       <c r="C50" s="11"/>
@@ -2693,8 +2743,9 @@
       <c r="Y50" s="15"/>
       <c r="Z50" s="15"/>
       <c r="AA50" s="16"/>
-    </row>
-    <row r="51" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB50" s="10"/>
+    </row>
+    <row r="51" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
       <c r="B51" s="10"/>
       <c r="C51" s="11"/>
@@ -2722,8 +2773,9 @@
       <c r="Y51" s="15"/>
       <c r="Z51" s="15"/>
       <c r="AA51" s="16"/>
-    </row>
-    <row r="52" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB51" s="10"/>
+    </row>
+    <row r="52" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
       <c r="B52" s="10"/>
       <c r="C52" s="11"/>
@@ -2751,8 +2803,9 @@
       <c r="Y52" s="15"/>
       <c r="Z52" s="15"/>
       <c r="AA52" s="16"/>
-    </row>
-    <row r="53" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB52" s="10"/>
+    </row>
+    <row r="53" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
       <c r="B53" s="10"/>
       <c r="C53" s="11"/>
@@ -2780,8 +2833,9 @@
       <c r="Y53" s="15"/>
       <c r="Z53" s="15"/>
       <c r="AA53" s="16"/>
-    </row>
-    <row r="54" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB53" s="10"/>
+    </row>
+    <row r="54" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="9"/>
       <c r="B54" s="10"/>
       <c r="C54" s="11"/>
@@ -2809,8 +2863,9 @@
       <c r="Y54" s="15"/>
       <c r="Z54" s="15"/>
       <c r="AA54" s="16"/>
-    </row>
-    <row r="55" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB54" s="10"/>
+    </row>
+    <row r="55" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="9"/>
       <c r="B55" s="10"/>
       <c r="C55" s="11"/>
@@ -2838,8 +2893,9 @@
       <c r="Y55" s="15"/>
       <c r="Z55" s="15"/>
       <c r="AA55" s="16"/>
-    </row>
-    <row r="56" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB55" s="10"/>
+    </row>
+    <row r="56" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="9"/>
       <c r="B56" s="10"/>
       <c r="C56" s="11"/>
@@ -2867,8 +2923,9 @@
       <c r="Y56" s="15"/>
       <c r="Z56" s="15"/>
       <c r="AA56" s="16"/>
-    </row>
-    <row r="57" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB56" s="10"/>
+    </row>
+    <row r="57" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="9"/>
       <c r="B57" s="10"/>
       <c r="C57" s="11"/>
@@ -2896,8 +2953,9 @@
       <c r="Y57" s="15"/>
       <c r="Z57" s="15"/>
       <c r="AA57" s="16"/>
-    </row>
-    <row r="58" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB57" s="10"/>
+    </row>
+    <row r="58" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="9"/>
       <c r="B58" s="10"/>
       <c r="C58" s="11"/>
@@ -2925,8 +2983,9 @@
       <c r="Y58" s="15"/>
       <c r="Z58" s="15"/>
       <c r="AA58" s="16"/>
-    </row>
-    <row r="59" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB58" s="10"/>
+    </row>
+    <row r="59" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="9"/>
       <c r="B59" s="10"/>
       <c r="C59" s="11"/>
@@ -2954,8 +3013,9 @@
       <c r="Y59" s="15"/>
       <c r="Z59" s="15"/>
       <c r="AA59" s="16"/>
-    </row>
-    <row r="60" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB59" s="10"/>
+    </row>
+    <row r="60" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="9"/>
       <c r="B60" s="10"/>
       <c r="C60" s="11"/>
@@ -2983,8 +3043,9 @@
       <c r="Y60" s="15"/>
       <c r="Z60" s="15"/>
       <c r="AA60" s="16"/>
-    </row>
-    <row r="61" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB60" s="10"/>
+    </row>
+    <row r="61" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="9"/>
       <c r="B61" s="10"/>
       <c r="C61" s="11"/>
@@ -3012,8 +3073,9 @@
       <c r="Y61" s="15"/>
       <c r="Z61" s="15"/>
       <c r="AA61" s="16"/>
-    </row>
-    <row r="62" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB61" s="10"/>
+    </row>
+    <row r="62" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="9"/>
       <c r="B62" s="10"/>
       <c r="C62" s="11"/>
@@ -3041,8 +3103,9 @@
       <c r="Y62" s="15"/>
       <c r="Z62" s="15"/>
       <c r="AA62" s="16"/>
-    </row>
-    <row r="63" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB62" s="10"/>
+    </row>
+    <row r="63" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="9"/>
       <c r="B63" s="10"/>
       <c r="C63" s="11"/>
@@ -3070,8 +3133,9 @@
       <c r="Y63" s="15"/>
       <c r="Z63" s="15"/>
       <c r="AA63" s="16"/>
-    </row>
-    <row r="64" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB63" s="10"/>
+    </row>
+    <row r="64" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="9"/>
       <c r="B64" s="10"/>
       <c r="C64" s="11"/>
@@ -3099,8 +3163,9 @@
       <c r="Y64" s="15"/>
       <c r="Z64" s="15"/>
       <c r="AA64" s="16"/>
-    </row>
-    <row r="65" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB64" s="10"/>
+    </row>
+    <row r="65" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="9"/>
       <c r="B65" s="10"/>
       <c r="C65" s="11"/>
@@ -3128,8 +3193,9 @@
       <c r="Y65" s="15"/>
       <c r="Z65" s="15"/>
       <c r="AA65" s="16"/>
-    </row>
-    <row r="66" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB65" s="10"/>
+    </row>
+    <row r="66" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="9"/>
       <c r="B66" s="10"/>
       <c r="C66" s="11"/>
@@ -3157,8 +3223,9 @@
       <c r="Y66" s="15"/>
       <c r="Z66" s="15"/>
       <c r="AA66" s="16"/>
-    </row>
-    <row r="67" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB66" s="10"/>
+    </row>
+    <row r="67" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="9"/>
       <c r="B67" s="10"/>
       <c r="C67" s="11"/>
@@ -3186,8 +3253,9 @@
       <c r="Y67" s="15"/>
       <c r="Z67" s="15"/>
       <c r="AA67" s="16"/>
-    </row>
-    <row r="68" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB67" s="10"/>
+    </row>
+    <row r="68" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="9"/>
       <c r="B68" s="10"/>
       <c r="C68" s="11"/>
@@ -3215,8 +3283,9 @@
       <c r="Y68" s="15"/>
       <c r="Z68" s="15"/>
       <c r="AA68" s="16"/>
-    </row>
-    <row r="69" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB68" s="10"/>
+    </row>
+    <row r="69" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="9"/>
       <c r="B69" s="10"/>
       <c r="C69" s="11"/>
@@ -3244,8 +3313,9 @@
       <c r="Y69" s="15"/>
       <c r="Z69" s="15"/>
       <c r="AA69" s="16"/>
-    </row>
-    <row r="70" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB69" s="10"/>
+    </row>
+    <row r="70" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="9"/>
       <c r="B70" s="10"/>
       <c r="C70" s="11"/>
@@ -3273,8 +3343,9 @@
       <c r="Y70" s="15"/>
       <c r="Z70" s="15"/>
       <c r="AA70" s="16"/>
-    </row>
-    <row r="71" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB70" s="10"/>
+    </row>
+    <row r="71" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="9"/>
       <c r="B71" s="10"/>
       <c r="C71" s="11"/>
@@ -3302,8 +3373,9 @@
       <c r="Y71" s="15"/>
       <c r="Z71" s="15"/>
       <c r="AA71" s="16"/>
-    </row>
-    <row r="72" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB71" s="10"/>
+    </row>
+    <row r="72" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="9"/>
       <c r="B72" s="10"/>
       <c r="C72" s="11"/>
@@ -3331,8 +3403,9 @@
       <c r="Y72" s="15"/>
       <c r="Z72" s="15"/>
       <c r="AA72" s="16"/>
-    </row>
-    <row r="73" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB72" s="10"/>
+    </row>
+    <row r="73" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="9"/>
       <c r="B73" s="10"/>
       <c r="C73" s="11"/>
@@ -3360,8 +3433,9 @@
       <c r="Y73" s="15"/>
       <c r="Z73" s="15"/>
       <c r="AA73" s="16"/>
-    </row>
-    <row r="74" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB73" s="10"/>
+    </row>
+    <row r="74" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="9"/>
       <c r="B74" s="10"/>
       <c r="C74" s="11"/>
@@ -3389,8 +3463,9 @@
       <c r="Y74" s="15"/>
       <c r="Z74" s="15"/>
       <c r="AA74" s="16"/>
-    </row>
-    <row r="75" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB74" s="10"/>
+    </row>
+    <row r="75" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="9"/>
       <c r="B75" s="10"/>
       <c r="C75" s="11"/>
@@ -3418,8 +3493,9 @@
       <c r="Y75" s="15"/>
       <c r="Z75" s="15"/>
       <c r="AA75" s="16"/>
-    </row>
-    <row r="76" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB75" s="10"/>
+    </row>
+    <row r="76" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="9"/>
       <c r="B76" s="10"/>
       <c r="C76" s="11"/>
@@ -3447,8 +3523,9 @@
       <c r="Y76" s="15"/>
       <c r="Z76" s="15"/>
       <c r="AA76" s="16"/>
-    </row>
-    <row r="77" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB76" s="10"/>
+    </row>
+    <row r="77" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="9"/>
       <c r="B77" s="10"/>
       <c r="C77" s="11"/>
@@ -3476,8 +3553,9 @@
       <c r="Y77" s="15"/>
       <c r="Z77" s="15"/>
       <c r="AA77" s="16"/>
-    </row>
-    <row r="78" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB77" s="10"/>
+    </row>
+    <row r="78" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="9"/>
       <c r="B78" s="10"/>
       <c r="C78" s="11"/>
@@ -3505,8 +3583,9 @@
       <c r="Y78" s="15"/>
       <c r="Z78" s="15"/>
       <c r="AA78" s="16"/>
-    </row>
-    <row r="79" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB78" s="10"/>
+    </row>
+    <row r="79" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="9"/>
       <c r="B79" s="10"/>
       <c r="C79" s="11"/>
@@ -3534,8 +3613,9 @@
       <c r="Y79" s="15"/>
       <c r="Z79" s="15"/>
       <c r="AA79" s="16"/>
-    </row>
-    <row r="80" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB79" s="10"/>
+    </row>
+    <row r="80" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="9"/>
       <c r="B80" s="10"/>
       <c r="C80" s="11"/>
@@ -3563,8 +3643,9 @@
       <c r="Y80" s="15"/>
       <c r="Z80" s="15"/>
       <c r="AA80" s="16"/>
-    </row>
-    <row r="81" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB80" s="10"/>
+    </row>
+    <row r="81" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="9"/>
       <c r="B81" s="10"/>
       <c r="C81" s="11"/>
@@ -3592,8 +3673,9 @@
       <c r="Y81" s="15"/>
       <c r="Z81" s="15"/>
       <c r="AA81" s="16"/>
-    </row>
-    <row r="82" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB81" s="10"/>
+    </row>
+    <row r="82" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="9"/>
       <c r="B82" s="10"/>
       <c r="C82" s="11"/>
@@ -3621,8 +3703,9 @@
       <c r="Y82" s="15"/>
       <c r="Z82" s="15"/>
       <c r="AA82" s="16"/>
-    </row>
-    <row r="83" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB82" s="10"/>
+    </row>
+    <row r="83" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="9"/>
       <c r="B83" s="10"/>
       <c r="C83" s="11"/>
@@ -3650,8 +3733,9 @@
       <c r="Y83" s="15"/>
       <c r="Z83" s="15"/>
       <c r="AA83" s="16"/>
-    </row>
-    <row r="84" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB83" s="10"/>
+    </row>
+    <row r="84" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="9"/>
       <c r="B84" s="10"/>
       <c r="C84" s="11"/>
@@ -3679,8 +3763,9 @@
       <c r="Y84" s="15"/>
       <c r="Z84" s="15"/>
       <c r="AA84" s="16"/>
-    </row>
-    <row r="85" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB84" s="10"/>
+    </row>
+    <row r="85" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="9"/>
       <c r="B85" s="10"/>
       <c r="C85" s="11"/>
@@ -3708,8 +3793,9 @@
       <c r="Y85" s="15"/>
       <c r="Z85" s="15"/>
       <c r="AA85" s="16"/>
-    </row>
-    <row r="86" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB85" s="10"/>
+    </row>
+    <row r="86" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="9"/>
       <c r="B86" s="10"/>
       <c r="C86" s="11"/>
@@ -3737,8 +3823,9 @@
       <c r="Y86" s="15"/>
       <c r="Z86" s="15"/>
       <c r="AA86" s="16"/>
-    </row>
-    <row r="87" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB86" s="10"/>
+    </row>
+    <row r="87" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="9"/>
       <c r="B87" s="10"/>
       <c r="C87" s="11"/>
@@ -3766,8 +3853,9 @@
       <c r="Y87" s="15"/>
       <c r="Z87" s="15"/>
       <c r="AA87" s="16"/>
-    </row>
-    <row r="88" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB87" s="10"/>
+    </row>
+    <row r="88" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="9"/>
       <c r="B88" s="10"/>
       <c r="C88" s="11"/>
@@ -3795,8 +3883,9 @@
       <c r="Y88" s="15"/>
       <c r="Z88" s="15"/>
       <c r="AA88" s="16"/>
-    </row>
-    <row r="89" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB88" s="10"/>
+    </row>
+    <row r="89" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="9"/>
       <c r="B89" s="10"/>
       <c r="C89" s="11"/>
@@ -3824,8 +3913,9 @@
       <c r="Y89" s="15"/>
       <c r="Z89" s="15"/>
       <c r="AA89" s="16"/>
-    </row>
-    <row r="90" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB89" s="10"/>
+    </row>
+    <row r="90" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="9"/>
       <c r="B90" s="10"/>
       <c r="C90" s="11"/>
@@ -3853,8 +3943,9 @@
       <c r="Y90" s="15"/>
       <c r="Z90" s="15"/>
       <c r="AA90" s="16"/>
-    </row>
-    <row r="91" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB90" s="10"/>
+    </row>
+    <row r="91" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="9"/>
       <c r="B91" s="10"/>
       <c r="C91" s="11"/>
@@ -3882,8 +3973,9 @@
       <c r="Y91" s="15"/>
       <c r="Z91" s="15"/>
       <c r="AA91" s="16"/>
-    </row>
-    <row r="92" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB91" s="10"/>
+    </row>
+    <row r="92" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="9"/>
       <c r="B92" s="10"/>
       <c r="C92" s="11"/>
@@ -3911,8 +4003,9 @@
       <c r="Y92" s="15"/>
       <c r="Z92" s="15"/>
       <c r="AA92" s="16"/>
-    </row>
-    <row r="93" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB92" s="10"/>
+    </row>
+    <row r="93" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="9"/>
       <c r="B93" s="10"/>
       <c r="C93" s="11"/>
@@ -3940,8 +4033,9 @@
       <c r="Y93" s="15"/>
       <c r="Z93" s="15"/>
       <c r="AA93" s="16"/>
-    </row>
-    <row r="94" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB93" s="10"/>
+    </row>
+    <row r="94" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="9"/>
       <c r="B94" s="10"/>
       <c r="C94" s="11"/>
@@ -3969,8 +4063,9 @@
       <c r="Y94" s="15"/>
       <c r="Z94" s="15"/>
       <c r="AA94" s="16"/>
-    </row>
-    <row r="95" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB94" s="10"/>
+    </row>
+    <row r="95" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="9"/>
       <c r="B95" s="10"/>
       <c r="C95" s="11"/>
@@ -3998,8 +4093,9 @@
       <c r="Y95" s="15"/>
       <c r="Z95" s="15"/>
       <c r="AA95" s="16"/>
-    </row>
-    <row r="96" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB95" s="10"/>
+    </row>
+    <row r="96" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="9"/>
       <c r="B96" s="10"/>
       <c r="C96" s="11"/>
@@ -4027,8 +4123,9 @@
       <c r="Y96" s="15"/>
       <c r="Z96" s="15"/>
       <c r="AA96" s="16"/>
-    </row>
-    <row r="97" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB96" s="10"/>
+    </row>
+    <row r="97" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="9"/>
       <c r="B97" s="10"/>
       <c r="C97" s="11"/>
@@ -4056,8 +4153,9 @@
       <c r="Y97" s="15"/>
       <c r="Z97" s="15"/>
       <c r="AA97" s="16"/>
-    </row>
-    <row r="98" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB97" s="10"/>
+    </row>
+    <row r="98" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="9"/>
       <c r="B98" s="10"/>
       <c r="C98" s="11"/>
@@ -4085,8 +4183,9 @@
       <c r="Y98" s="15"/>
       <c r="Z98" s="15"/>
       <c r="AA98" s="16"/>
-    </row>
-    <row r="99" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB98" s="10"/>
+    </row>
+    <row r="99" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="9"/>
       <c r="B99" s="10"/>
       <c r="C99" s="11"/>
@@ -4114,8 +4213,9 @@
       <c r="Y99" s="15"/>
       <c r="Z99" s="15"/>
       <c r="AA99" s="16"/>
-    </row>
-    <row r="100" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB99" s="10"/>
+    </row>
+    <row r="100" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="9"/>
       <c r="B100" s="10"/>
       <c r="C100" s="11"/>
@@ -4143,8 +4243,9 @@
       <c r="Y100" s="15"/>
       <c r="Z100" s="15"/>
       <c r="AA100" s="16"/>
-    </row>
-    <row r="101" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB100" s="10"/>
+    </row>
+    <row r="101" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="9"/>
       <c r="B101" s="10"/>
       <c r="C101" s="11"/>
@@ -4172,8 +4273,9 @@
       <c r="Y101" s="15"/>
       <c r="Z101" s="15"/>
       <c r="AA101" s="16"/>
-    </row>
-    <row r="102" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB101" s="10"/>
+    </row>
+    <row r="102" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="9"/>
       <c r="B102" s="10"/>
       <c r="C102" s="11"/>
@@ -4201,8 +4303,9 @@
       <c r="Y102" s="15"/>
       <c r="Z102" s="15"/>
       <c r="AA102" s="16"/>
-    </row>
-    <row r="103" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB102" s="10"/>
+    </row>
+    <row r="103" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="9"/>
       <c r="B103" s="10"/>
       <c r="C103" s="11"/>
@@ -4230,8 +4333,9 @@
       <c r="Y103" s="15"/>
       <c r="Z103" s="15"/>
       <c r="AA103" s="16"/>
-    </row>
-    <row r="104" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB103" s="10"/>
+    </row>
+    <row r="104" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="9"/>
       <c r="B104" s="10"/>
       <c r="C104" s="11"/>
@@ -4259,8 +4363,9 @@
       <c r="Y104" s="15"/>
       <c r="Z104" s="15"/>
       <c r="AA104" s="16"/>
-    </row>
-    <row r="105" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB104" s="10"/>
+    </row>
+    <row r="105" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="9"/>
       <c r="B105" s="10"/>
       <c r="C105" s="11"/>
@@ -4288,8 +4393,9 @@
       <c r="Y105" s="15"/>
       <c r="Z105" s="15"/>
       <c r="AA105" s="16"/>
-    </row>
-    <row r="106" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB105" s="10"/>
+    </row>
+    <row r="106" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="9"/>
       <c r="B106" s="10"/>
       <c r="C106" s="11"/>
@@ -4317,8 +4423,9 @@
       <c r="Y106" s="15"/>
       <c r="Z106" s="15"/>
       <c r="AA106" s="16"/>
-    </row>
-    <row r="107" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB106" s="10"/>
+    </row>
+    <row r="107" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="9"/>
       <c r="B107" s="10"/>
       <c r="C107" s="11"/>
@@ -4346,8 +4453,9 @@
       <c r="Y107" s="15"/>
       <c r="Z107" s="15"/>
       <c r="AA107" s="16"/>
-    </row>
-    <row r="108" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB107" s="10"/>
+    </row>
+    <row r="108" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="9"/>
       <c r="B108" s="10"/>
       <c r="C108" s="11"/>
@@ -4375,8 +4483,9 @@
       <c r="Y108" s="15"/>
       <c r="Z108" s="15"/>
       <c r="AA108" s="16"/>
-    </row>
-    <row r="109" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB108" s="10"/>
+    </row>
+    <row r="109" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="9"/>
       <c r="B109" s="10"/>
       <c r="C109" s="11"/>
@@ -4404,8 +4513,9 @@
       <c r="Y109" s="15"/>
       <c r="Z109" s="15"/>
       <c r="AA109" s="16"/>
-    </row>
-    <row r="110" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB109" s="10"/>
+    </row>
+    <row r="110" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="9"/>
       <c r="B110" s="10"/>
       <c r="C110" s="11"/>
@@ -4433,8 +4543,9 @@
       <c r="Y110" s="15"/>
       <c r="Z110" s="15"/>
       <c r="AA110" s="16"/>
-    </row>
-    <row r="111" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB110" s="10"/>
+    </row>
+    <row r="111" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="9"/>
       <c r="B111" s="10"/>
       <c r="C111" s="11"/>
@@ -4462,8 +4573,9 @@
       <c r="Y111" s="15"/>
       <c r="Z111" s="15"/>
       <c r="AA111" s="16"/>
-    </row>
-    <row r="112" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB111" s="10"/>
+    </row>
+    <row r="112" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="9"/>
       <c r="B112" s="10"/>
       <c r="C112" s="11"/>
@@ -4491,8 +4603,9 @@
       <c r="Y112" s="15"/>
       <c r="Z112" s="15"/>
       <c r="AA112" s="16"/>
-    </row>
-    <row r="113" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB112" s="10"/>
+    </row>
+    <row r="113" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="9"/>
       <c r="B113" s="10"/>
       <c r="C113" s="11"/>
@@ -4520,8 +4633,9 @@
       <c r="Y113" s="15"/>
       <c r="Z113" s="15"/>
       <c r="AA113" s="16"/>
-    </row>
-    <row r="114" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB113" s="10"/>
+    </row>
+    <row r="114" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="9"/>
       <c r="B114" s="10"/>
       <c r="C114" s="11"/>
@@ -4549,8 +4663,9 @@
       <c r="Y114" s="15"/>
       <c r="Z114" s="15"/>
       <c r="AA114" s="16"/>
-    </row>
-    <row r="115" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB114" s="10"/>
+    </row>
+    <row r="115" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="9"/>
       <c r="B115" s="10"/>
       <c r="C115" s="11"/>
@@ -4578,8 +4693,9 @@
       <c r="Y115" s="15"/>
       <c r="Z115" s="15"/>
       <c r="AA115" s="16"/>
-    </row>
-    <row r="116" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB115" s="10"/>
+    </row>
+    <row r="116" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="9"/>
       <c r="B116" s="10"/>
       <c r="C116" s="11"/>
@@ -4607,8 +4723,9 @@
       <c r="Y116" s="15"/>
       <c r="Z116" s="15"/>
       <c r="AA116" s="16"/>
-    </row>
-    <row r="117" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB116" s="10"/>
+    </row>
+    <row r="117" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="9"/>
       <c r="B117" s="10"/>
       <c r="C117" s="11"/>
@@ -4636,8 +4753,9 @@
       <c r="Y117" s="15"/>
       <c r="Z117" s="15"/>
       <c r="AA117" s="16"/>
-    </row>
-    <row r="118" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB117" s="10"/>
+    </row>
+    <row r="118" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="9"/>
       <c r="B118" s="10"/>
       <c r="C118" s="11"/>
@@ -4665,8 +4783,9 @@
       <c r="Y118" s="15"/>
       <c r="Z118" s="15"/>
       <c r="AA118" s="16"/>
-    </row>
-    <row r="119" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB118" s="10"/>
+    </row>
+    <row r="119" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="9"/>
       <c r="B119" s="10"/>
       <c r="C119" s="11"/>
@@ -4694,8 +4813,9 @@
       <c r="Y119" s="15"/>
       <c r="Z119" s="15"/>
       <c r="AA119" s="16"/>
-    </row>
-    <row r="120" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB119" s="10"/>
+    </row>
+    <row r="120" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="9"/>
       <c r="B120" s="10"/>
       <c r="C120" s="11"/>
@@ -4723,8 +4843,9 @@
       <c r="Y120" s="15"/>
       <c r="Z120" s="15"/>
       <c r="AA120" s="16"/>
-    </row>
-    <row r="121" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB120" s="10"/>
+    </row>
+    <row r="121" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="9"/>
       <c r="B121" s="10"/>
       <c r="C121" s="11"/>
@@ -4752,8 +4873,9 @@
       <c r="Y121" s="15"/>
       <c r="Z121" s="15"/>
       <c r="AA121" s="16"/>
-    </row>
-    <row r="122" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB121" s="10"/>
+    </row>
+    <row r="122" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="9"/>
       <c r="B122" s="10"/>
       <c r="C122" s="11"/>
@@ -4781,8 +4903,9 @@
       <c r="Y122" s="15"/>
       <c r="Z122" s="15"/>
       <c r="AA122" s="16"/>
-    </row>
-    <row r="123" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB122" s="10"/>
+    </row>
+    <row r="123" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="9"/>
       <c r="B123" s="10"/>
       <c r="C123" s="11"/>
@@ -4810,8 +4933,9 @@
       <c r="Y123" s="15"/>
       <c r="Z123" s="15"/>
       <c r="AA123" s="16"/>
-    </row>
-    <row r="124" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB123" s="10"/>
+    </row>
+    <row r="124" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="9"/>
       <c r="B124" s="10"/>
       <c r="C124" s="11"/>
@@ -4839,8 +4963,9 @@
       <c r="Y124" s="15"/>
       <c r="Z124" s="15"/>
       <c r="AA124" s="16"/>
-    </row>
-    <row r="125" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB124" s="10"/>
+    </row>
+    <row r="125" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="9"/>
       <c r="B125" s="10"/>
       <c r="C125" s="11"/>
@@ -4868,8 +4993,9 @@
       <c r="Y125" s="15"/>
       <c r="Z125" s="15"/>
       <c r="AA125" s="16"/>
-    </row>
-    <row r="126" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB125" s="10"/>
+    </row>
+    <row r="126" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="9"/>
       <c r="B126" s="10"/>
       <c r="C126" s="11"/>
@@ -4897,8 +5023,9 @@
       <c r="Y126" s="15"/>
       <c r="Z126" s="15"/>
       <c r="AA126" s="16"/>
-    </row>
-    <row r="127" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB126" s="10"/>
+    </row>
+    <row r="127" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="9"/>
       <c r="B127" s="10"/>
       <c r="C127" s="11"/>
@@ -4926,8 +5053,9 @@
       <c r="Y127" s="15"/>
       <c r="Z127" s="15"/>
       <c r="AA127" s="16"/>
-    </row>
-    <row r="128" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB127" s="10"/>
+    </row>
+    <row r="128" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="9"/>
       <c r="B128" s="10"/>
       <c r="C128" s="11"/>
@@ -4955,8 +5083,9 @@
       <c r="Y128" s="15"/>
       <c r="Z128" s="15"/>
       <c r="AA128" s="16"/>
-    </row>
-    <row r="129" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB128" s="10"/>
+    </row>
+    <row r="129" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="9"/>
       <c r="B129" s="10"/>
       <c r="C129" s="11"/>
@@ -4984,8 +5113,9 @@
       <c r="Y129" s="15"/>
       <c r="Z129" s="15"/>
       <c r="AA129" s="16"/>
-    </row>
-    <row r="130" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB129" s="10"/>
+    </row>
+    <row r="130" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="9"/>
       <c r="B130" s="10"/>
       <c r="C130" s="11"/>
@@ -5013,8 +5143,9 @@
       <c r="Y130" s="15"/>
       <c r="Z130" s="15"/>
       <c r="AA130" s="16"/>
-    </row>
-    <row r="131" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB130" s="10"/>
+    </row>
+    <row r="131" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="9"/>
       <c r="B131" s="10"/>
       <c r="C131" s="11"/>
@@ -5042,8 +5173,9 @@
       <c r="Y131" s="15"/>
       <c r="Z131" s="15"/>
       <c r="AA131" s="16"/>
-    </row>
-    <row r="132" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB131" s="10"/>
+    </row>
+    <row r="132" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="9"/>
       <c r="B132" s="10"/>
       <c r="C132" s="11"/>
@@ -5071,8 +5203,9 @@
       <c r="Y132" s="15"/>
       <c r="Z132" s="15"/>
       <c r="AA132" s="16"/>
-    </row>
-    <row r="133" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB132" s="10"/>
+    </row>
+    <row r="133" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="9"/>
       <c r="B133" s="10"/>
       <c r="C133" s="11"/>
@@ -5100,8 +5233,9 @@
       <c r="Y133" s="15"/>
       <c r="Z133" s="15"/>
       <c r="AA133" s="16"/>
-    </row>
-    <row r="134" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB133" s="10"/>
+    </row>
+    <row r="134" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A134" s="9"/>
       <c r="B134" s="10"/>
       <c r="C134" s="11"/>
@@ -5129,8 +5263,9 @@
       <c r="Y134" s="15"/>
       <c r="Z134" s="15"/>
       <c r="AA134" s="16"/>
-    </row>
-    <row r="135" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB134" s="10"/>
+    </row>
+    <row r="135" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A135" s="9"/>
       <c r="B135" s="10"/>
       <c r="C135" s="11"/>
@@ -5158,8 +5293,9 @@
       <c r="Y135" s="15"/>
       <c r="Z135" s="15"/>
       <c r="AA135" s="16"/>
-    </row>
-    <row r="136" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB135" s="10"/>
+    </row>
+    <row r="136" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="9"/>
       <c r="B136" s="10"/>
       <c r="C136" s="11"/>
@@ -5187,8 +5323,9 @@
       <c r="Y136" s="15"/>
       <c r="Z136" s="15"/>
       <c r="AA136" s="16"/>
-    </row>
-    <row r="137" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB136" s="10"/>
+    </row>
+    <row r="137" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="9"/>
       <c r="B137" s="10"/>
       <c r="C137" s="11"/>
@@ -5216,8 +5353,9 @@
       <c r="Y137" s="15"/>
       <c r="Z137" s="15"/>
       <c r="AA137" s="16"/>
-    </row>
-    <row r="138" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB137" s="10"/>
+    </row>
+    <row r="138" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="9"/>
       <c r="B138" s="10"/>
       <c r="C138" s="11"/>
@@ -5269,8 +5407,9 @@
       <c r="AA138" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="139" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB138" s="10"/>
+    </row>
+    <row r="139" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="9"/>
       <c r="B139" s="10"/>
       <c r="C139" s="11"/>
@@ -5322,8 +5461,9 @@
       <c r="AA139" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="140" spans="1:27" s="17" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="AB139" s="10"/>
+    </row>
+    <row r="140" spans="1:28" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="9"/>
       <c r="B140" s="10"/>
       <c r="C140" s="11"/>
@@ -5375,8 +5515,9 @@
       <c r="AA140" s="16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="AB140" s="10"/>
+    </row>
+    <row r="141" spans="1:28" x14ac:dyDescent="0.15">
       <c r="D141" s="18"/>
       <c r="E141" s="18"/>
       <c r="F141" s="18"/>
@@ -5396,33 +5537,33 @@
       <c r="T141" s="19"/>
       <c r="U141" s="19"/>
     </row>
-    <row r="142" spans="1:27" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B142" s="38" t="s">
+    <row r="142" spans="1:28" ht="18" x14ac:dyDescent="0.15">
+      <c r="B142" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C142" s="38"/>
-      <c r="D142" s="38"/>
-      <c r="E142" s="38"/>
-      <c r="F142" s="38"/>
-      <c r="G142" s="38"/>
-      <c r="H142" s="38"/>
-      <c r="I142" s="38"/>
-      <c r="J142" s="38"/>
-    </row>
-    <row r="143" spans="1:27" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B143" s="38" t="s">
+      <c r="C142" s="40"/>
+      <c r="D142" s="40"/>
+      <c r="E142" s="40"/>
+      <c r="F142" s="40"/>
+      <c r="G142" s="40"/>
+      <c r="H142" s="40"/>
+      <c r="I142" s="40"/>
+      <c r="J142" s="40"/>
+    </row>
+    <row r="143" spans="1:28" ht="18" x14ac:dyDescent="0.15">
+      <c r="B143" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C143" s="38"/>
-      <c r="D143" s="38"/>
-      <c r="E143" s="38"/>
-      <c r="F143" s="38"/>
-      <c r="G143" s="38"/>
-      <c r="H143" s="38"/>
-      <c r="I143" s="38"/>
-      <c r="J143" s="38"/>
-    </row>
-    <row r="144" spans="1:27" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="C143" s="40"/>
+      <c r="D143" s="40"/>
+      <c r="E143" s="40"/>
+      <c r="F143" s="40"/>
+      <c r="G143" s="40"/>
+      <c r="H143" s="40"/>
+      <c r="I143" s="40"/>
+      <c r="J143" s="40"/>
+    </row>
+    <row r="144" spans="1:28" ht="17" x14ac:dyDescent="0.15">
       <c r="A144" s="20"/>
       <c r="B144" s="21"/>
       <c r="C144" s="20"/>
@@ -5434,250 +5575,254 @@
       <c r="I144" s="20"/>
       <c r="J144" s="23"/>
       <c r="K144" s="23"/>
-      <c r="Q144" s="39" t="s">
+      <c r="Q144" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="R144" s="40"/>
-      <c r="S144" s="40"/>
-      <c r="T144" s="41"/>
-      <c r="U144" s="39" t="s">
+      <c r="R144" s="42"/>
+      <c r="S144" s="42"/>
+      <c r="T144" s="43"/>
+      <c r="U144" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="V144" s="40"/>
-      <c r="W144" s="41"/>
-      <c r="X144" s="48" t="s">
+      <c r="V144" s="42"/>
+      <c r="W144" s="43"/>
+      <c r="X144" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="Y144" s="49"/>
-      <c r="Z144" s="50"/>
-    </row>
-    <row r="145" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y144" s="51"/>
+      <c r="Z144" s="52"/>
+    </row>
+    <row r="145" spans="2:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B145" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="Q145" s="42"/>
-      <c r="R145" s="43"/>
-      <c r="S145" s="43"/>
-      <c r="T145" s="44"/>
-      <c r="U145" s="42"/>
-      <c r="V145" s="43"/>
-      <c r="W145" s="44"/>
-      <c r="X145" s="51"/>
-      <c r="Y145" s="52"/>
-      <c r="Z145" s="53"/>
-    </row>
-    <row r="146" spans="2:26" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q145" s="44"/>
+      <c r="R145" s="45"/>
+      <c r="S145" s="45"/>
+      <c r="T145" s="46"/>
+      <c r="U145" s="44"/>
+      <c r="V145" s="45"/>
+      <c r="W145" s="46"/>
+      <c r="X145" s="53"/>
+      <c r="Y145" s="54"/>
+      <c r="Z145" s="55"/>
+    </row>
+    <row r="146" spans="2:26" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="B146" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="Q146" s="42"/>
-      <c r="R146" s="43"/>
-      <c r="S146" s="43"/>
-      <c r="T146" s="44"/>
-      <c r="U146" s="42"/>
-      <c r="V146" s="43"/>
-      <c r="W146" s="44"/>
-      <c r="X146" s="51"/>
-      <c r="Y146" s="52"/>
-      <c r="Z146" s="53"/>
-    </row>
-    <row r="147" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q146" s="44"/>
+      <c r="R146" s="45"/>
+      <c r="S146" s="45"/>
+      <c r="T146" s="46"/>
+      <c r="U146" s="44"/>
+      <c r="V146" s="45"/>
+      <c r="W146" s="46"/>
+      <c r="X146" s="53"/>
+      <c r="Y146" s="54"/>
+      <c r="Z146" s="55"/>
+    </row>
+    <row r="147" spans="2:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B147" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q147" s="42"/>
-      <c r="R147" s="43"/>
-      <c r="S147" s="43"/>
-      <c r="T147" s="44"/>
-      <c r="U147" s="42"/>
-      <c r="V147" s="43"/>
-      <c r="W147" s="44"/>
-      <c r="X147" s="51"/>
-      <c r="Y147" s="52"/>
-      <c r="Z147" s="53"/>
-    </row>
-    <row r="148" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q147" s="44"/>
+      <c r="R147" s="45"/>
+      <c r="S147" s="45"/>
+      <c r="T147" s="46"/>
+      <c r="U147" s="44"/>
+      <c r="V147" s="45"/>
+      <c r="W147" s="46"/>
+      <c r="X147" s="53"/>
+      <c r="Y147" s="54"/>
+      <c r="Z147" s="55"/>
+    </row>
+    <row r="148" spans="2:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B148" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="Q148" s="45"/>
-      <c r="R148" s="46"/>
-      <c r="S148" s="46"/>
-      <c r="T148" s="47"/>
-      <c r="U148" s="45"/>
-      <c r="V148" s="46"/>
-      <c r="W148" s="47"/>
-      <c r="X148" s="54"/>
-      <c r="Y148" s="55"/>
-      <c r="Z148" s="56"/>
-    </row>
-    <row r="149" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q148" s="47"/>
+      <c r="R148" s="48"/>
+      <c r="S148" s="48"/>
+      <c r="T148" s="49"/>
+      <c r="U148" s="47"/>
+      <c r="V148" s="48"/>
+      <c r="W148" s="49"/>
+      <c r="X148" s="56"/>
+      <c r="Y148" s="57"/>
+      <c r="Z148" s="58"/>
+    </row>
+    <row r="149" spans="2:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B149" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="Q149" s="32" t="s">
+      <c r="Q149" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="R149" s="32"/>
-      <c r="S149" s="32"/>
-      <c r="T149" s="32"/>
-      <c r="U149" s="32" t="s">
+      <c r="R149" s="33"/>
+      <c r="S149" s="33"/>
+      <c r="T149" s="33"/>
+      <c r="U149" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="V149" s="32"/>
-      <c r="W149" s="32"/>
-      <c r="X149" s="33" t="s">
+      <c r="V149" s="33"/>
+      <c r="W149" s="33"/>
+      <c r="X149" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="Y149" s="33"/>
-      <c r="Z149" s="33"/>
-    </row>
-    <row r="150" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y149" s="34"/>
+      <c r="Z149" s="34"/>
+    </row>
+    <row r="150" spans="2:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B150" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="Q150" s="32"/>
-      <c r="R150" s="32"/>
-      <c r="S150" s="32"/>
-      <c r="T150" s="32"/>
-      <c r="U150" s="32"/>
-      <c r="V150" s="32"/>
-      <c r="W150" s="32"/>
-      <c r="X150" s="33"/>
-      <c r="Y150" s="33"/>
-      <c r="Z150" s="33"/>
-    </row>
-    <row r="151" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q150" s="33"/>
+      <c r="R150" s="33"/>
+      <c r="S150" s="33"/>
+      <c r="T150" s="33"/>
+      <c r="U150" s="33"/>
+      <c r="V150" s="33"/>
+      <c r="W150" s="33"/>
+      <c r="X150" s="34"/>
+      <c r="Y150" s="34"/>
+      <c r="Z150" s="34"/>
+    </row>
+    <row r="151" spans="2:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B151" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="Q151" s="32"/>
-      <c r="R151" s="32"/>
-      <c r="S151" s="32"/>
-      <c r="T151" s="32"/>
-      <c r="U151" s="32"/>
-      <c r="V151" s="32"/>
-      <c r="W151" s="32"/>
-      <c r="X151" s="33"/>
-      <c r="Y151" s="33"/>
-      <c r="Z151" s="33"/>
-    </row>
-    <row r="152" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q151" s="33"/>
+      <c r="R151" s="33"/>
+      <c r="S151" s="33"/>
+      <c r="T151" s="33"/>
+      <c r="U151" s="33"/>
+      <c r="V151" s="33"/>
+      <c r="W151" s="33"/>
+      <c r="X151" s="34"/>
+      <c r="Y151" s="34"/>
+      <c r="Z151" s="34"/>
+    </row>
+    <row r="152" spans="2:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B152" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="Q152" s="57"/>
-      <c r="R152" s="57"/>
-      <c r="S152" s="57"/>
-      <c r="T152" s="57"/>
-      <c r="U152" s="57"/>
-      <c r="V152" s="57"/>
-      <c r="W152" s="57"/>
-      <c r="X152" s="58"/>
-      <c r="Y152" s="58"/>
-      <c r="Z152" s="58"/>
-    </row>
-    <row r="153" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q152" s="29"/>
+      <c r="R152" s="29"/>
+      <c r="S152" s="29"/>
+      <c r="T152" s="29"/>
+      <c r="U152" s="29"/>
+      <c r="V152" s="29"/>
+      <c r="W152" s="29"/>
+      <c r="X152" s="30"/>
+      <c r="Y152" s="30"/>
+      <c r="Z152" s="30"/>
+    </row>
+    <row r="153" spans="2:26" ht="16" x14ac:dyDescent="0.2">
       <c r="B153" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="Q153" s="57"/>
-      <c r="R153" s="57"/>
-      <c r="S153" s="57"/>
-      <c r="T153" s="57"/>
-      <c r="U153" s="57"/>
-      <c r="V153" s="57"/>
-      <c r="W153" s="57"/>
-      <c r="X153" s="58"/>
-      <c r="Y153" s="58"/>
-      <c r="Z153" s="58"/>
-    </row>
-    <row r="154" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="Q154" s="57"/>
-      <c r="R154" s="57"/>
-      <c r="S154" s="57"/>
-      <c r="T154" s="57"/>
-      <c r="U154" s="57"/>
-      <c r="V154" s="57"/>
-      <c r="W154" s="57"/>
-      <c r="X154" s="58"/>
-      <c r="Y154" s="58"/>
-      <c r="Z154" s="58"/>
-    </row>
-    <row r="155" spans="2:26" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q155" s="57"/>
-      <c r="R155" s="57"/>
-      <c r="S155" s="57"/>
-      <c r="T155" s="57"/>
-      <c r="U155" s="57"/>
-      <c r="V155" s="57"/>
-      <c r="W155" s="57"/>
-      <c r="X155" s="58"/>
-      <c r="Y155" s="58"/>
-      <c r="Z155" s="58"/>
-    </row>
-    <row r="156" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="Q156" s="57"/>
-      <c r="R156" s="57"/>
-      <c r="S156" s="57"/>
-      <c r="T156" s="57"/>
-      <c r="U156" s="57"/>
-      <c r="V156" s="57"/>
-      <c r="W156" s="57"/>
-      <c r="X156" s="58"/>
-      <c r="Y156" s="58"/>
-      <c r="Z156" s="58"/>
-    </row>
-    <row r="157" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="Q157" s="57"/>
-      <c r="R157" s="57"/>
-      <c r="S157" s="57"/>
-      <c r="T157" s="57"/>
-      <c r="U157" s="57"/>
-      <c r="V157" s="57"/>
-      <c r="W157" s="57"/>
-      <c r="X157" s="58"/>
-      <c r="Y157" s="58"/>
-      <c r="Z157" s="58"/>
-    </row>
-    <row r="158" spans="2:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="Q158" s="59" t="s">
+      <c r="Q153" s="29"/>
+      <c r="R153" s="29"/>
+      <c r="S153" s="29"/>
+      <c r="T153" s="29"/>
+      <c r="U153" s="29"/>
+      <c r="V153" s="29"/>
+      <c r="W153" s="29"/>
+      <c r="X153" s="30"/>
+      <c r="Y153" s="30"/>
+      <c r="Z153" s="30"/>
+    </row>
+    <row r="154" spans="2:26" x14ac:dyDescent="0.15">
+      <c r="Q154" s="29"/>
+      <c r="R154" s="29"/>
+      <c r="S154" s="29"/>
+      <c r="T154" s="29"/>
+      <c r="U154" s="29"/>
+      <c r="V154" s="29"/>
+      <c r="W154" s="29"/>
+      <c r="X154" s="30"/>
+      <c r="Y154" s="30"/>
+      <c r="Z154" s="30"/>
+    </row>
+    <row r="155" spans="2:26" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q155" s="29"/>
+      <c r="R155" s="29"/>
+      <c r="S155" s="29"/>
+      <c r="T155" s="29"/>
+      <c r="U155" s="29"/>
+      <c r="V155" s="29"/>
+      <c r="W155" s="29"/>
+      <c r="X155" s="30"/>
+      <c r="Y155" s="30"/>
+      <c r="Z155" s="30"/>
+    </row>
+    <row r="156" spans="2:26" x14ac:dyDescent="0.15">
+      <c r="Q156" s="29"/>
+      <c r="R156" s="29"/>
+      <c r="S156" s="29"/>
+      <c r="T156" s="29"/>
+      <c r="U156" s="29"/>
+      <c r="V156" s="29"/>
+      <c r="W156" s="29"/>
+      <c r="X156" s="30"/>
+      <c r="Y156" s="30"/>
+      <c r="Z156" s="30"/>
+    </row>
+    <row r="157" spans="2:26" x14ac:dyDescent="0.15">
+      <c r="Q157" s="29"/>
+      <c r="R157" s="29"/>
+      <c r="S157" s="29"/>
+      <c r="T157" s="29"/>
+      <c r="U157" s="29"/>
+      <c r="V157" s="29"/>
+      <c r="W157" s="29"/>
+      <c r="X157" s="30"/>
+      <c r="Y157" s="30"/>
+      <c r="Z157" s="30"/>
+    </row>
+    <row r="158" spans="2:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="Q158" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="R158" s="59"/>
-      <c r="S158" s="59"/>
-      <c r="T158" s="59"/>
-      <c r="U158" s="59" t="s">
+      <c r="R158" s="31"/>
+      <c r="S158" s="31"/>
+      <c r="T158" s="31"/>
+      <c r="U158" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="V158" s="59"/>
-      <c r="W158" s="59"/>
-      <c r="X158" s="60" t="s">
+      <c r="V158" s="31"/>
+      <c r="W158" s="31"/>
+      <c r="X158" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="Y158" s="60"/>
-      <c r="Z158" s="60"/>
-    </row>
-    <row r="159" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="Q159" s="59"/>
-      <c r="R159" s="59"/>
-      <c r="S159" s="59"/>
-      <c r="T159" s="59"/>
-      <c r="U159" s="59"/>
-      <c r="V159" s="59"/>
-      <c r="W159" s="59"/>
-      <c r="X159" s="60"/>
-      <c r="Y159" s="60"/>
-      <c r="Z159" s="60"/>
+      <c r="Y158" s="32"/>
+      <c r="Z158" s="32"/>
+    </row>
+    <row r="159" spans="2:26" x14ac:dyDescent="0.15">
+      <c r="Q159" s="31"/>
+      <c r="R159" s="31"/>
+      <c r="S159" s="31"/>
+      <c r="T159" s="31"/>
+      <c r="U159" s="31"/>
+      <c r="V159" s="31"/>
+      <c r="W159" s="31"/>
+      <c r="X159" s="32"/>
+      <c r="Y159" s="32"/>
+      <c r="Z159" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="Q152:T157"/>
-    <mergeCell ref="U152:W157"/>
-    <mergeCell ref="X152:Z157"/>
-    <mergeCell ref="Q158:T159"/>
-    <mergeCell ref="U158:W159"/>
-    <mergeCell ref="X158:Z159"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:Z4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
     <mergeCell ref="Q149:T151"/>
     <mergeCell ref="U149:W151"/>
     <mergeCell ref="X149:Z151"/>
@@ -5691,16 +5836,12 @@
     <mergeCell ref="Q144:T148"/>
     <mergeCell ref="U144:W148"/>
     <mergeCell ref="X144:Z148"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A4:Z4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="Q152:T157"/>
+    <mergeCell ref="U152:W157"/>
+    <mergeCell ref="X152:Z157"/>
+    <mergeCell ref="Q158:T159"/>
+    <mergeCell ref="U158:W159"/>
+    <mergeCell ref="X158:Z159"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>